<commit_message>
DEI-3-3 Added data model sketch
</commit_message>
<xml_diff>
--- a/data_eng_instructions._planning.xlsx
+++ b/data_eng_instructions._planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarasvaranovich/Desktop/JOB_REL/Attempt_1/Interviews/Johnson&amp;Johnson/task/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4718DF-5E61-554C-9122-02149F656F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C7BA18-F543-CC4D-A1E5-4B0208B9626C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="640" windowWidth="28040" windowHeight="17180" xr2:uid="{327C4E5F-3208-1446-8C84-88A26933E71F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
   <si>
     <t>Number</t>
   </si>
@@ -198,13 +198,40 @@
   </si>
   <si>
     <t>Deadline:</t>
+  </si>
+  <si>
+    <t>TODO</t>
+  </si>
+  <si>
+    <t>DEI-0</t>
+  </si>
+  <si>
+    <t>Tech debt:</t>
+  </si>
+  <si>
+    <t>udf</t>
+  </si>
+  <si>
+    <t>apply appropriate names (classes, utils, tests)</t>
+  </si>
+  <si>
+    <t>50 min</t>
+  </si>
+  <si>
+    <t>5 min</t>
+  </si>
+  <si>
+    <t>parametrise queries impliying big data</t>
+  </si>
+  <si>
+    <t>10 min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -223,6 +250,13 @@
       <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -246,11 +280,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD16672-586C-6145-AF10-08CB5050EC7A}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="191" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -644,6 +680,9 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
+      <c r="B3" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="C3" t="s">
         <v>37</v>
       </c>
@@ -658,6 +697,9 @@
       <c r="A4" t="s">
         <v>18</v>
       </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
       <c r="C4" t="s">
         <v>38</v>
       </c>
@@ -672,6 +714,9 @@
       <c r="A5" t="s">
         <v>19</v>
       </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
       <c r="C5" t="s">
         <v>39</v>
       </c>
@@ -686,6 +731,9 @@
       <c r="A6" t="s">
         <v>20</v>
       </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
       <c r="C6" t="s">
         <v>40</v>
       </c>
@@ -700,6 +748,9 @@
       <c r="A7" t="s">
         <v>21</v>
       </c>
+      <c r="B7" t="s">
+        <v>62</v>
+      </c>
       <c r="C7" t="s">
         <v>41</v>
       </c>
@@ -714,6 +765,9 @@
       <c r="A8" t="s">
         <v>22</v>
       </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
       <c r="C8" t="s">
         <v>42</v>
       </c>
@@ -728,6 +782,9 @@
       <c r="A9" t="s">
         <v>28</v>
       </c>
+      <c r="B9" s="2">
+        <v>20</v>
+      </c>
       <c r="C9" t="s">
         <v>43</v>
       </c>
@@ -823,17 +880,39 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
       <c r="F16" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
       <c r="E17" s="2" t="s">
         <v>53</v>
       </c>
       <c r="F17" s="3">
         <v>46042</v>
       </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
DEI-3-3 Added DWH model diagram
</commit_message>
<xml_diff>
--- a/data_eng_instructions._planning.xlsx
+++ b/data_eng_instructions._planning.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarasvaranovich/Desktop/JOB_REL/Attempt_1/Interviews/Johnson&amp;Johnson/task/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarasvaranovich/Desktop/JOB_REL/Attempt_1/Interviews/Johnson&amp;Johnson/data_eng_instructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C7BA18-F543-CC4D-A1E5-4B0208B9626C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0385F93-792B-0C4C-B4C8-3C3E0AB130BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="640" windowWidth="28040" windowHeight="17180" xr2:uid="{327C4E5F-3208-1446-8C84-88A26933E71F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
   <si>
     <t>Number</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>10 min</t>
+  </si>
+  <si>
+    <t>Check defects, check defects and downtime. Check states</t>
+  </si>
+  <si>
+    <t>3 h</t>
   </si>
 </sst>
 </file>
@@ -624,7 +630,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="191" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -808,10 +814,16 @@
       <c r="F10" t="s">
         <v>50</v>
       </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>64</v>
       </c>
       <c r="C11" t="s">
         <v>45</v>

</xml_diff>

<commit_message>
DEI-3-1 Manufacturing factory reader not tested
</commit_message>
<xml_diff>
--- a/data_eng_instructions._planning.xlsx
+++ b/data_eng_instructions._planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarasvaranovich/Desktop/JOB_REL/Attempt_1/Interviews/Johnson&amp;Johnson/data_eng_instructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0385F93-792B-0C4C-B4C8-3C3E0AB130BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F26D815-B844-4D4B-BC65-48D4D585EF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="640" windowWidth="28040" windowHeight="17180" xr2:uid="{327C4E5F-3208-1446-8C84-88A26933E71F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
   <si>
     <t>Number</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>3 h</t>
+  </si>
+  <si>
+    <t>(16-00)20</t>
   </si>
 </sst>
 </file>
@@ -630,7 +633,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="191" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,8 +791,8 @@
       <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2">
-        <v>20</v>
+      <c r="B9" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="C9" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
DEI-3-1 Refactored - added parent class for reader
</commit_message>
<xml_diff>
--- a/data_eng_instructions._planning.xlsx
+++ b/data_eng_instructions._planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarasvaranovich/Desktop/JOB_REL/Attempt_1/Interviews/Johnson&amp;Johnson/data_eng_instructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F26D815-B844-4D4B-BC65-48D4D585EF9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE4DCD7-7714-A846-AF8D-4561F4A73AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="640" windowWidth="28040" windowHeight="17180" xr2:uid="{327C4E5F-3208-1446-8C84-88A26933E71F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
   <si>
     <t>Number</t>
   </si>
@@ -233,7 +233,10 @@
     <t>3 h</t>
   </si>
   <si>
-    <t>(16-00)20</t>
+    <t>2 hour 20 min</t>
+  </si>
+  <si>
+    <t>18-15</t>
   </si>
 </sst>
 </file>
@@ -632,12 +635,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD16672-586C-6145-AF10-08CB5050EC7A}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="191" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="4" max="4" width="28.1640625" customWidth="1"/>
   </cols>
@@ -791,7 +795,7 @@
       <c r="A9" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" t="s">
         <v>65</v>
       </c>
       <c r="C9" t="s">
@@ -807,6 +811,9 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>29</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C10" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
DEI-3-2 Defect filter - test failed
</commit_message>
<xml_diff>
--- a/data_eng_instructions._planning.xlsx
+++ b/data_eng_instructions._planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarasvaranovich/Desktop/JOB_REL/Attempt_1/Interviews/Johnson&amp;Johnson/data_eng_instructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE4DCD7-7714-A846-AF8D-4561F4A73AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034CBFDC-DB97-BA48-8B1D-4167A453C67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="640" windowWidth="28040" windowHeight="17180" xr2:uid="{327C4E5F-3208-1446-8C84-88A26933E71F}"/>
   </bookViews>
@@ -236,7 +236,7 @@
     <t>2 hour 20 min</t>
   </si>
   <si>
-    <t>18-15</t>
+    <t>2 hour 5 min</t>
   </si>
 </sst>
 </file>
@@ -292,13 +292,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -636,7 +637,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -812,7 +813,7 @@
       <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>66</v>
       </c>
       <c r="C10" t="s">

</xml_diff>

<commit_message>
DEI-3-2 Added invalid defects definitions filter transform
</commit_message>
<xml_diff>
--- a/data_eng_instructions._planning.xlsx
+++ b/data_eng_instructions._planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarasvaranovich/Desktop/JOB_REL/Attempt_1/Interviews/Johnson&amp;Johnson/data_eng_instructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034CBFDC-DB97-BA48-8B1D-4167A453C67C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417C845C-442A-5846-B10E-491DFDFFB811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="640" windowWidth="28040" windowHeight="17180" xr2:uid="{327C4E5F-3208-1446-8C84-88A26933E71F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
   <si>
     <t>Number</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>2 hour 5 min</t>
+  </si>
+  <si>
+    <t>40 min</t>
   </si>
 </sst>
 </file>
@@ -637,7 +640,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -822,6 +825,9 @@
       <c r="D10" t="s">
         <v>24</v>
       </c>
+      <c r="E10" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="F10" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
DEI-3-4 Implemented generic writer
</commit_message>
<xml_diff>
--- a/data_eng_instructions._planning.xlsx
+++ b/data_eng_instructions._planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarasvaranovich/Desktop/JOB_REL/Attempt_1/Interviews/Johnson&amp;Johnson/data_eng_instructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417C845C-442A-5846-B10E-491DFDFFB811}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8F63BF-2D5C-D740-99DD-B84B0D2173AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="640" windowWidth="28040" windowHeight="17180" xr2:uid="{327C4E5F-3208-1446-8C84-88A26933E71F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
   <si>
     <t>Number</t>
   </si>
@@ -236,10 +236,7 @@
     <t>2 hour 20 min</t>
   </si>
   <si>
-    <t>2 hour 5 min</t>
-  </si>
-  <si>
-    <t>40 min</t>
+    <t>2 hour 40 min</t>
   </si>
 </sst>
 </file>
@@ -639,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD16672-586C-6145-AF10-08CB5050EC7A}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="191" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="191" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -825,9 +822,7 @@
       <c r="D10" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>67</v>
-      </c>
+      <c r="E10" s="2"/>
       <c r="F10" t="s">
         <v>50</v>
       </c>

</xml_diff>